<commit_message>
630	Replace adj_color_table with vector;
843.386s
</commit_message>
<xml_diff>
--- a/npbenchmark-main/tabucol_vector/tabu_result.xlsx
+++ b/npbenchmark-main/tabucol_vector/tabu_result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\npbenchmark\npbenchmark-main\tabucol_vector\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C40343F-8138-4406-810E-633C66AD74F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9981C24-92E4-46D2-BD88-13331F05E795}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
   <si>
     <t>Seed</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -49,6 +49,10 @@
   </si>
   <si>
     <t>vector</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vector&lt;int&gt; tabu_tenure_table_i</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -380,10 +384,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -427,106 +431,117 @@
       <c r="B3">
         <v>1</v>
       </c>
+      <c r="C3" s="2">
+        <v>123604301</v>
+      </c>
       <c r="D3" s="1">
         <v>92.239099999999993</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4" s="2">
-        <v>91729575</v>
+      <c r="A4" t="s">
+        <v>6</v>
       </c>
       <c r="D4" s="1">
-        <v>76.668999999999997</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B5">
-        <v>3</v>
-      </c>
-      <c r="C5" s="2">
-        <v>119326345</v>
-      </c>
-      <c r="D5" s="1">
-        <v>96.628500000000003</v>
+        <v>843.38599999999997</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C6" s="2">
-        <v>78869859</v>
+        <v>91729575</v>
       </c>
       <c r="D6" s="1">
-        <v>64.704800000000006</v>
+        <v>76.668999999999997</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C7" s="2">
-        <v>258364945</v>
+        <v>119326345</v>
       </c>
       <c r="D7" s="1">
-        <v>212.17099999999999</v>
+        <v>96.628500000000003</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C8" s="2">
-        <v>312726838</v>
+        <v>78869859</v>
       </c>
       <c r="D8" s="1">
-        <v>256.678</v>
+        <v>64.704800000000006</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C9" s="2">
-        <v>32209388</v>
+        <v>258364945</v>
       </c>
       <c r="D9" s="1">
-        <v>28.588799999999999</v>
+        <v>212.17099999999999</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C10" s="2">
-        <v>107452109</v>
+        <v>312726838</v>
       </c>
       <c r="D10" s="1">
-        <v>88.991900000000001</v>
+        <v>256.678</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C11" s="2">
-        <v>417779635</v>
+        <v>32209388</v>
       </c>
       <c r="D11" s="1">
-        <v>321.54300000000001</v>
+        <v>28.588799999999999</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12">
+        <v>8</v>
+      </c>
+      <c r="C12" s="2">
+        <v>107452109</v>
+      </c>
+      <c r="D12" s="1">
+        <v>88.991900000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>9</v>
+      </c>
+      <c r="C13" s="2">
+        <v>417779635</v>
+      </c>
+      <c r="D13" s="1">
+        <v>321.54300000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B14">
         <v>10</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C14" s="2">
         <v>28009744</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D14" s="1">
         <v>23.5991</v>
       </c>
     </row>

</xml_diff>

<commit_message>
replace 2d vector with struct
</commit_message>
<xml_diff>
--- a/npbenchmark-main/tabucol_vector/tabu_result.xlsx
+++ b/npbenchmark-main/tabucol_vector/tabu_result.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\npbenchmark\npbenchmark-main\tabucol_vector\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78525BED-55AD-4F86-81AD-67820F0B5EB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD8AAC4-AD62-418C-A679-33D15313E408}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="500.1" sheetId="1" r:id="rId1"/>
     <sheet name="500.5" sheetId="2" r:id="rId2"/>
     <sheet name="500.9" sheetId="3" r:id="rId3"/>
+    <sheet name="variables" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="25">
   <si>
     <t>Seed</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -75,6 +76,66 @@
   </si>
   <si>
     <t>yuanFang_reduce</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int num_vertex;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int num_color</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vector&lt;vector&lt;int&gt;&gt; adj_list</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vector&lt;int&gt; vertex_edge_num</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vector&lt;int&gt; single_solution</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int conflict</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int best_conflict</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vector&lt;vector&lt;long long int&gt;&gt; tabu_tenure_table</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vector&lt;vector&lt;int&gt;&gt; adj_color_table</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int min_delta</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int node_moved</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int color_moved</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>long long int iter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vector&lt;vector&lt;int&gt;&gt; equal_nontabu_delta</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vector&lt;vector&lt;int&gt;&gt; equal_tabu_delta</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -410,8 +471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -759,6 +820,15 @@
       <c r="B29">
         <v>1</v>
       </c>
+      <c r="C29" s="2">
+        <v>172805497</v>
+      </c>
+      <c r="D29" s="1">
+        <v>388.80200000000002</v>
+      </c>
+      <c r="E29" s="2">
+        <v>444456</v>
+      </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
@@ -767,6 +837,15 @@
       <c r="B30">
         <v>2</v>
       </c>
+      <c r="C30" s="2">
+        <v>51180986</v>
+      </c>
+      <c r="D30" s="1">
+        <v>122.26600000000001</v>
+      </c>
+      <c r="E30" s="2">
+        <v>418605</v>
+      </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
@@ -774,6 +853,15 @@
       </c>
       <c r="B31">
         <v>3</v>
+      </c>
+      <c r="C31" s="2">
+        <v>164547891</v>
+      </c>
+      <c r="D31" s="1">
+        <v>375.36</v>
+      </c>
+      <c r="E31" s="2">
+        <v>438373</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -841,15 +929,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECD6EFFC-BA4E-4954-8C8C-5C7E8E2EF2DD}">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.21875" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" customWidth="1"/>
     <col min="3" max="3" width="14.88671875" style="2" customWidth="1"/>
     <col min="4" max="4" width="8.88671875" style="1"/>
     <col min="5" max="5" width="10" style="3" customWidth="1"/>
@@ -1165,6 +1253,113 @@
         <v>10</v>
       </c>
       <c r="E23" s="2"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26" s="2">
+        <v>14288454</v>
+      </c>
+      <c r="D26" s="1">
+        <v>233.97300000000001</v>
+      </c>
+      <c r="E26" s="3">
+        <v>61068.9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>9</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27" s="2">
+        <v>112114436</v>
+      </c>
+      <c r="D27" s="1">
+        <v>1795.97</v>
+      </c>
+      <c r="E27" s="3">
+        <v>62425.599999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>9</v>
+      </c>
+      <c r="B28">
+        <v>3</v>
+      </c>
+      <c r="C28" s="2">
+        <v>195040707</v>
+      </c>
+      <c r="D28" s="1">
+        <v>3059.37</v>
+      </c>
+      <c r="E28" s="3">
+        <v>63751.9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>9</v>
+      </c>
+      <c r="B30">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>9</v>
+      </c>
+      <c r="B31">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>9</v>
+      </c>
+      <c r="B32">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>9</v>
+      </c>
+      <c r="B33">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>9</v>
+      </c>
+      <c r="B34">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>9</v>
+      </c>
+      <c r="B35">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1439,4 +1634,103 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F4E3E9D-78F1-4185-B13B-18A9A4AD65AB}">
+  <dimension ref="A1:A16"/>
+  <sheetViews>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="49.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
242	Combine node_moved and color_moved with moved
</commit_message>
<xml_diff>
--- a/npbenchmark-main/tabucol_vector/tabu_result.xlsx
+++ b/npbenchmark-main/tabucol_vector/tabu_result.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\npbenchmark\npbenchmark-main\tabucol_vector\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD8AAC4-AD62-418C-A679-33D15313E408}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DE5A8A1-B61D-4603-B736-B41D0F2F65FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="500.1" sheetId="1" r:id="rId1"/>
@@ -131,11 +131,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>vector&lt;vector&lt;int&gt;&gt; equal_nontabu_delta</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>vector&lt;vector&lt;int&gt;&gt; equal_tabu_delta</t>
+    <t>vector&lt;Move&gt; equal_nontabu_delta</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vector&lt;Move&gt; equal_tabu_delta</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -931,7 +931,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECD6EFFC-BA4E-4954-8C8C-5C7E8E2EF2DD}">
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
@@ -1640,7 +1640,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F4E3E9D-78F1-4185-B13B-18A9A4AD65AB}">
   <dimension ref="A1:A16"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
@@ -1732,5 +1732,6 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
replace some int with unsigned
</commit_message>
<xml_diff>
--- a/npbenchmark-main/tabucol_vector/tabu_result.xlsx
+++ b/npbenchmark-main/tabucol_vector/tabu_result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\npbenchmark\npbenchmark-main\tabucol_vector\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DE5A8A1-B61D-4603-B736-B41D0F2F65FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C571473-DF5C-4779-9DAE-52AF6BC74C33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="24">
   <si>
     <t>Seed</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -119,14 +119,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>int node_moved</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>int color_moved</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>long long int iter</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -136,6 +128,10 @@
   </si>
   <si>
     <t>vector&lt;Move&gt; equal_tabu_delta</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Move moved</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1638,7 +1634,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F4E3E9D-78F1-4185-B13B-18A9A4AD65AB}">
-  <dimension ref="A1:A16"/>
+  <dimension ref="A1:A15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="A17" sqref="A17"/>
@@ -1706,27 +1702,22 @@
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
245	Change node_moved and color_moved back
</commit_message>
<xml_diff>
--- a/npbenchmark-main/tabucol_vector/tabu_result.xlsx
+++ b/npbenchmark-main/tabucol_vector/tabu_result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\npbenchmark\npbenchmark-main\tabucol_vector\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95D7B287-8572-4CFC-8633-4DD848C74037}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4E56B1E-E982-4FE2-B487-2B732723E2AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="43">
   <si>
     <t>Seed</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -157,6 +157,548 @@
   <si>
     <t>int get_solution(int i);</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">int </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF660E7A"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>num_vertex</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF080808"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">int </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF660E7A"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>num_color</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF080808"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>vector</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF080808"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF008080"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>VerNode</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF080808"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF660E7A"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>adj_list</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF080808"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>vector</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF080808"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF008080"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>vector</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF080808"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0033B3"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>int</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF080808"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">&gt;&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF660E7A"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>adj_color_table</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF080808"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>vector</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF080808"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF008080"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>vector</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF080808"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0033B3"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>long long int</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF080808"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">&gt;&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF660E7A"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>tabu_tenure_table</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF080808"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">int </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF660E7A"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>best_conflict</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF080808"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">int </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF660E7A"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>conflict</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF080808"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">int </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF660E7A"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>conflict_num</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF080808"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>vector</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF080808"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0033B3"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>int</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF080808"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF660E7A"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>conflicts</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF080808"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>vector</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF080808"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0033B3"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>int</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF080808"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF660E7A"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>conflict_index</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF080808"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">int </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF660E7A"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>num_population</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF080808"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>vector</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF080808"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF008080"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>vector</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF080808"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0033B3"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>unsigned int</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF080808"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">&gt;&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF660E7A"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>solution_collection</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF080808"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>vector</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF080808"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF008080"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>Population_solution</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF080808"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF660E7A"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>population_solution</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF080808"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>;</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -168,7 +710,7 @@
     <numFmt numFmtId="177" formatCode="#,##0_ "/>
     <numFmt numFmtId="178" formatCode="#,##0_);[Red]\(#,##0\)"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -182,6 +724,30 @@
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF080808"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0033B3"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF660E7A"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF008080"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -204,11 +770,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -495,7 +1067,7 @@
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col min="1" max="1" width="16.77734375" customWidth="1"/>
     <col min="3" max="3" width="13.88671875" style="2" customWidth="1"/>
@@ -503,7 +1075,7 @@
     <col min="5" max="5" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -520,7 +1092,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -538,7 +1110,7 @@
         <v>1230652.7509508354</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -556,7 +1128,7 @@
         <v>1340042.3573083433</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -564,7 +1136,7 @@
         <v>843.38599999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -582,7 +1154,7 @@
         <v>1196436.3041124835</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -600,7 +1172,7 @@
         <v>1234898.0373285315</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -618,7 +1190,7 @@
         <v>1218918.2100864232</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -636,7 +1208,7 @@
         <v>1217720.3529228782</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -654,7 +1226,7 @@
         <v>1218362.4541254023</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -672,7 +1244,7 @@
         <v>1126643.5807029326</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -690,7 +1262,7 @@
         <v>1207436.9577455926</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -708,7 +1280,7 @@
         <v>1299296.31495632</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -726,7 +1298,7 @@
         <v>1186898.822412719</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -743,7 +1315,7 @@
         <v>983741</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -760,7 +1332,7 @@
         <v>943455</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -777,7 +1349,7 @@
         <v>982032</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>8</v>
       </c>
@@ -785,7 +1357,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -793,7 +1365,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>8</v>
       </c>
@@ -801,7 +1373,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
         <v>8</v>
       </c>
@@ -809,7 +1381,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -817,7 +1389,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
         <v>8</v>
       </c>
@@ -825,7 +1397,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
         <v>8</v>
       </c>
@@ -833,7 +1405,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5">
       <c r="A29" t="s">
         <v>9</v>
       </c>
@@ -850,7 +1422,7 @@
         <v>444456</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5">
       <c r="A30" t="s">
         <v>9</v>
       </c>
@@ -867,7 +1439,7 @@
         <v>418605</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5">
       <c r="A31" t="s">
         <v>9</v>
       </c>
@@ -884,7 +1456,7 @@
         <v>438373</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5">
       <c r="A32" t="s">
         <v>9</v>
       </c>
@@ -892,7 +1464,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2">
       <c r="A33" t="s">
         <v>9</v>
       </c>
@@ -900,7 +1472,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2">
       <c r="A34" t="s">
         <v>9</v>
       </c>
@@ -908,7 +1480,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2">
       <c r="A35" t="s">
         <v>9</v>
       </c>
@@ -916,7 +1488,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2">
       <c r="A36" t="s">
         <v>9</v>
       </c>
@@ -924,7 +1496,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2">
       <c r="A37" t="s">
         <v>9</v>
       </c>
@@ -932,7 +1504,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2">
       <c r="A38" t="s">
         <v>9</v>
       </c>
@@ -955,7 +1527,7 @@
       <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col min="1" max="1" width="17.6640625" customWidth="1"/>
     <col min="3" max="3" width="14.88671875" style="2" customWidth="1"/>
@@ -963,7 +1535,7 @@
     <col min="5" max="5" width="10" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -980,7 +1552,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -998,7 +1570,7 @@
         <v>473273.25632831879</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1016,7 +1588,7 @@
         <v>445154.95802801318</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1034,7 +1606,7 @@
         <v>472001.5792604686</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1052,7 +1624,7 @@
         <v>472658.07587719942</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1070,7 +1642,7 @@
         <v>466346.70597423741</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1088,7 +1660,7 @@
         <v>436591.46054898959</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1106,7 +1678,7 @@
         <v>459256.36381774273</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1124,7 +1696,7 @@
         <v>473146.72833732649</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -1142,7 +1714,7 @@
         <v>473563.24185920745</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -1160,7 +1732,7 @@
         <v>466271.34876865178</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -1177,7 +1749,7 @@
         <v>289485</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -1194,7 +1766,7 @@
         <v>289000</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -1211,7 +1783,7 @@
         <v>287851</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -1220,7 +1792,7 @@
       </c>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -1229,7 +1801,7 @@
       </c>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -1238,7 +1810,7 @@
       </c>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>8</v>
       </c>
@@ -1247,7 +1819,7 @@
       </c>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -1256,7 +1828,7 @@
       </c>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>8</v>
       </c>
@@ -1265,7 +1837,7 @@
       </c>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
         <v>8</v>
       </c>
@@ -1274,7 +1846,7 @@
       </c>
       <c r="E23" s="2"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
         <v>9</v>
       </c>
@@ -1291,7 +1863,7 @@
         <v>61068.9</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
         <v>9</v>
       </c>
@@ -1308,7 +1880,7 @@
         <v>62425.599999999999</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
         <v>9</v>
       </c>
@@ -1325,7 +1897,7 @@
         <v>63751.9</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5">
       <c r="A29" t="s">
         <v>9</v>
       </c>
@@ -1333,7 +1905,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5">
       <c r="A30" t="s">
         <v>9</v>
       </c>
@@ -1341,7 +1913,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5">
       <c r="A31" t="s">
         <v>9</v>
       </c>
@@ -1349,7 +1921,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5">
       <c r="A32" t="s">
         <v>9</v>
       </c>
@@ -1357,7 +1929,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2">
       <c r="A33" t="s">
         <v>9</v>
       </c>
@@ -1365,7 +1937,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2">
       <c r="A34" t="s">
         <v>9</v>
       </c>
@@ -1373,7 +1945,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2">
       <c r="A35" t="s">
         <v>9</v>
       </c>
@@ -1396,14 +1968,14 @@
       <selection activeCell="C14" sqref="C14:E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col min="1" max="1" width="16.33203125" customWidth="1"/>
     <col min="3" max="3" width="13.109375" customWidth="1"/>
     <col min="5" max="5" width="11.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1420,7 +1992,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1431,7 +2003,7 @@
       <c r="D2" s="1"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1442,7 +2014,7 @@
       <c r="D3" s="1"/>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1453,7 +2025,7 @@
       <c r="D4" s="1"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1464,7 +2036,7 @@
       <c r="D5" s="1"/>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1475,7 +2047,7 @@
       <c r="D6" s="1"/>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1486,7 +2058,7 @@
       <c r="D7" s="1"/>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1497,7 +2069,7 @@
       <c r="D8" s="1"/>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1508,7 +2080,7 @@
       <c r="D9" s="1"/>
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -1519,7 +2091,7 @@
       <c r="D10" s="1"/>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -1530,17 +2102,17 @@
       <c r="D11" s="1"/>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="C12" s="2"/>
       <c r="D12" s="1"/>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="C13" s="2"/>
       <c r="D13" s="1"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -1551,7 +2123,7 @@
       <c r="D14" s="1"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -1562,7 +2134,7 @@
       <c r="D15" s="1"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -1573,7 +2145,7 @@
       <c r="D16" s="1"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -1584,7 +2156,7 @@
       <c r="D17" s="1"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -1595,7 +2167,7 @@
       <c r="D18" s="1"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -1606,7 +2178,7 @@
       <c r="D19" s="1"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>8</v>
       </c>
@@ -1617,7 +2189,7 @@
       <c r="D20" s="1"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -1628,7 +2200,7 @@
       <c r="D21" s="1"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>8</v>
       </c>
@@ -1639,7 +2211,7 @@
       <c r="D22" s="1"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
         <v>8</v>
       </c>
@@ -1658,119 +2230,183 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F4E3E9D-78F1-4185-B13B-18A9A4AD65AB}">
-  <dimension ref="A1:A22"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col min="1" max="1" width="49.88671875" customWidth="1"/>
+    <col min="2" max="2" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B3" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B4" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B5" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B8" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="B9" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="B10" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="B11" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="B12" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="B13" s="4"/>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="B14" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="B15" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="21" spans="1:2">
+      <c r="B21" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="B22" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="B23" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="B24" s="5"/>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="30" spans="1:2">
+      <c r="A30" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
change sequence of var
</commit_message>
<xml_diff>
--- a/npbenchmark-main/tabucol_vector/tabu_result.xlsx
+++ b/npbenchmark-main/tabucol_vector/tabu_result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\npbenchmark\npbenchmark-main\tabucol_vector\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABC92DF6-0547-413E-8E2A-47077A359A94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{054856B8-3FDC-4F6C-93FA-E679EB837225}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="46">
   <si>
     <t>Seed</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1409,6 +1409,129 @@
         <family val="2"/>
       </rPr>
       <t>();</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>vector</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF080808"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF008080"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>Move</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF080808"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF660E7A"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>tabu_move</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF080808"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>vector</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF080808"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF008080"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>Move</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF080808"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF660E7A"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>non_tabu_move</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF080808"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Move </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF660E7A"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>moved</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF080808"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>;</t>
     </r>
   </si>
 </sst>
@@ -2947,10 +3070,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F4E3E9D-78F1-4185-B13B-18A9A4AD65AB}">
-  <dimension ref="A1:B36"/>
+  <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -3044,27 +3167,23 @@
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="B14" s="4"/>
+      <c r="B14" s="5"/>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
+        <v>16</v>
+      </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="4" t="s">
@@ -3075,90 +3194,102 @@
       <c r="A19" s="5" t="s">
         <v>36</v>
       </c>
+      <c r="B19" s="5" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>25</v>
+      <c r="A20" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="5" t="s">
         <v>38</v>
       </c>
+      <c r="B21" s="5" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="5" t="s">
-        <v>39</v>
+      <c r="A22" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:2">
-      <c r="B23" s="4" t="s">
+      <c r="A23" s="5"/>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="B24" s="4" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="B24" s="5" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="B25" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="B26" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
-      <c r="B26" s="5"/>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28" t="s">
+    <row r="27" spans="1:2">
+      <c r="B27" s="5"/>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
         <v>11</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B29" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B32" s="4" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
-      <c r="B32" s="4" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="33" spans="2:2">
       <c r="B33" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2">
+      <c r="B34" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="2:2">
-      <c r="B34" s="4"/>
-    </row>
-    <row r="36" spans="2:2">
-      <c r="B36" s="4" t="s">
+    <row r="35" spans="2:2">
+      <c r="B35" s="4"/>
+    </row>
+    <row r="37" spans="2:2">
+      <c r="B37" s="4" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>

<commit_message>
261	Change sequence of tabucol.h
</commit_message>
<xml_diff>
--- a/npbenchmark-main/tabucol_vector/tabu_result.xlsx
+++ b/npbenchmark-main/tabucol_vector/tabu_result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\npbenchmark\npbenchmark-main\tabucol_vector\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{054856B8-3FDC-4F6C-93FA-E679EB837225}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F24F4D69-FB56-4864-8F39-878F14806CC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3070,10 +3070,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F4E3E9D-78F1-4185-B13B-18A9A4AD65AB}">
-  <dimension ref="A1:B37"/>
+  <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -3128,168 +3128,166 @@
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="5" t="s">
-        <v>34</v>
-      </c>
+      <c r="A7" s="5"/>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="5"/>
+      <c r="A8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="4" t="s">
-        <v>17</v>
-      </c>
       <c r="B10" s="4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="B11" s="4" t="s">
-        <v>19</v>
+      <c r="B11" s="5" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="B12" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="B13" s="5" t="s">
-        <v>21</v>
-      </c>
+      <c r="B13" s="5"/>
     </row>
     <row r="14" spans="1:2">
-      <c r="B14" s="5"/>
+      <c r="A14" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>16</v>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="4" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="4" t="s">
-        <v>35</v>
+      <c r="A18" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="5" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>44</v>
+      <c r="A21" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>25</v>
-      </c>
+      <c r="A22" s="5"/>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="5"/>
+      <c r="B23" s="4" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="24" spans="1:2">
-      <c r="B24" s="4" t="s">
-        <v>22</v>
+      <c r="A24" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="B25" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:2">
-      <c r="B26" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="B27" s="5"/>
+      <c r="B26" s="5"/>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
+        <v>11</v>
+      </c>
+      <c r="B28" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="29" spans="1:2">
-      <c r="A29" t="s">
-        <v>11</v>
-      </c>
-      <c r="B29" t="s">
-        <v>11</v>
+      <c r="A29" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="32" spans="1:2">
-      <c r="A32" s="4" t="s">
-        <v>42</v>
-      </c>
       <c r="B32" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="33" spans="2:2">
       <c r="B33" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="34" spans="2:2">
-      <c r="B34" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="35" spans="2:2">
-      <c r="B35" s="4"/>
-    </row>
-    <row r="37" spans="2:2">
-      <c r="B37" s="4" t="s">
+      <c r="B34" s="4"/>
+    </row>
+    <row r="36" spans="2:2">
+      <c r="B36" s="4" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>

<commit_message>
302	Remove unnecessary memset;
</commit_message>
<xml_diff>
--- a/npbenchmark-main/tabucol_vector/tabu_result.xlsx
+++ b/npbenchmark-main/tabucol_vector/tabu_result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\npbenchmark\npbenchmark-main\tabucol_vector\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9607135C-F241-4C55-9D99-C31520DCBA21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B573A656-928A-4854-9B17-C6AF5B961581}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2074,7 +2074,7 @@
   <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2549,7 +2549,7 @@
         <v>2</v>
       </c>
       <c r="D42" s="1">
-        <v>249.387</v>
+        <v>41</v>
       </c>
     </row>
     <row r="43" spans="1:4">

</xml_diff>

<commit_message>
305	Replace tabu_tenure_table with dynamic;
</commit_message>
<xml_diff>
--- a/npbenchmark-main/tabucol_vector/tabu_result.xlsx
+++ b/npbenchmark-main/tabucol_vector/tabu_result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\npbenchmark\npbenchmark-main\tabucol_vector\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDC691BC-7A00-45C2-A226-F9FB1E94E8DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24AC9018-D1EC-4C9F-867B-33650F55B8DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="55">
   <si>
     <t>Seed</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2083,10 +2083,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E61"/>
+  <dimension ref="A1:E85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D58" sqref="D58"/>
+    <sheetView tabSelected="1" topLeftCell="A59" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D79" sqref="D79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2756,6 +2756,211 @@
         <v>10</v>
       </c>
       <c r="C61" s="1"/>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" t="s">
+        <v>50</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D64" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" t="s">
+        <v>46</v>
+      </c>
+      <c r="B65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66" t="s">
+        <v>46</v>
+      </c>
+      <c r="B66">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67" t="s">
+        <v>46</v>
+      </c>
+      <c r="B67">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68" t="s">
+        <v>46</v>
+      </c>
+      <c r="B68">
+        <v>4</v>
+      </c>
+      <c r="C68" s="1"/>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69" t="s">
+        <v>46</v>
+      </c>
+      <c r="B69">
+        <v>5</v>
+      </c>
+      <c r="C69" s="1"/>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70" t="s">
+        <v>46</v>
+      </c>
+      <c r="B70">
+        <v>6</v>
+      </c>
+      <c r="C70" s="1"/>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71" t="s">
+        <v>46</v>
+      </c>
+      <c r="B71">
+        <v>7</v>
+      </c>
+      <c r="C71" s="1"/>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72" t="s">
+        <v>46</v>
+      </c>
+      <c r="B72">
+        <v>8</v>
+      </c>
+      <c r="C72" s="1"/>
+    </row>
+    <row r="73" spans="1:4">
+      <c r="A73" t="s">
+        <v>46</v>
+      </c>
+      <c r="B73">
+        <v>9</v>
+      </c>
+      <c r="C73" s="1"/>
+    </row>
+    <row r="74" spans="1:4">
+      <c r="A74" t="s">
+        <v>46</v>
+      </c>
+      <c r="B74">
+        <v>10</v>
+      </c>
+      <c r="C74" s="1"/>
+    </row>
+    <row r="75" spans="1:4">
+      <c r="A75" t="s">
+        <v>53</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D75" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
+      <c r="A76" t="s">
+        <v>46</v>
+      </c>
+      <c r="B76">
+        <v>1</v>
+      </c>
+      <c r="D76" s="1">
+        <v>37.597900000000003</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="A77" t="s">
+        <v>46</v>
+      </c>
+      <c r="B77">
+        <v>2</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
+      <c r="A78" t="s">
+        <v>46</v>
+      </c>
+      <c r="B78">
+        <v>3</v>
+      </c>
+      <c r="D78" s="1">
+        <v>27.9678</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
+      <c r="A79" t="s">
+        <v>46</v>
+      </c>
+      <c r="B79">
+        <v>4</v>
+      </c>
+      <c r="C79" s="1"/>
+    </row>
+    <row r="80" spans="1:4">
+      <c r="A80" t="s">
+        <v>46</v>
+      </c>
+      <c r="B80">
+        <v>5</v>
+      </c>
+      <c r="C80" s="1"/>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" t="s">
+        <v>46</v>
+      </c>
+      <c r="B81">
+        <v>6</v>
+      </c>
+      <c r="C81" s="1"/>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" t="s">
+        <v>46</v>
+      </c>
+      <c r="B82">
+        <v>7</v>
+      </c>
+      <c r="C82" s="1"/>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83" t="s">
+        <v>46</v>
+      </c>
+      <c r="B83">
+        <v>8</v>
+      </c>
+      <c r="C83" s="1"/>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84" t="s">
+        <v>46</v>
+      </c>
+      <c r="B84">
+        <v>9</v>
+      </c>
+      <c r="C84" s="1"/>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85" t="s">
+        <v>46</v>
+      </c>
+      <c r="B85">
+        <v>10</v>
+      </c>
+      <c r="C85" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
306	Replace adj_color_table with dynamic;
</commit_message>
<xml_diff>
--- a/npbenchmark-main/tabucol_vector/tabu_result.xlsx
+++ b/npbenchmark-main/tabucol_vector/tabu_result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\npbenchmark\npbenchmark-main\tabucol_vector\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24AC9018-D1EC-4C9F-867B-33650F55B8DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4378C1EB-4691-471E-ADA5-9C1DA5450904}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2085,8 +2085,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D79" sqref="D79"/>
+    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D77" sqref="D77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2874,7 +2874,7 @@
         <v>1</v>
       </c>
       <c r="D76" s="1">
-        <v>37.597900000000003</v>
+        <v>35.658999999999999</v>
       </c>
     </row>
     <row r="77" spans="1:4">

</xml_diff>

<commit_message>
309	Replace adj_list with dynamic;
</commit_message>
<xml_diff>
--- a/npbenchmark-main/tabucol_vector/tabu_result.xlsx
+++ b/npbenchmark-main/tabucol_vector/tabu_result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\npbenchmark\npbenchmark-main\tabucol_vector\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4378C1EB-4691-471E-ADA5-9C1DA5450904}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE9461D4-20EE-4728-BBB6-FA9ACAF60C29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2086,7 +2086,7 @@
   <dimension ref="A1:E85"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A56" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D77" sqref="D77"/>
+      <selection activeCell="D79" sqref="D79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2896,7 +2896,7 @@
         <v>3</v>
       </c>
       <c r="D78" s="1">
-        <v>27.9678</v>
+        <v>26.7226</v>
       </c>
     </row>
     <row r="79" spans="1:4">

</xml_diff>

<commit_message>
evaluate Line 4 and Line 5
</commit_message>
<xml_diff>
--- a/npbenchmark-main/tabucol_vector/tabu_result.xlsx
+++ b/npbenchmark-main/tabucol_vector/tabu_result.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\npbenchmark\npbenchmark-main\tabucol_vector\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BBD473D-7BAE-4744-9AC4-975B8192B56C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4133C0FA-0E49-4CE8-9571-BEFBD1017C4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="500.1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <sheet name="1000.9" sheetId="7" r:id="rId7"/>
     <sheet name="variables" sheetId="4" r:id="rId8"/>
     <sheet name="data_size" sheetId="8" r:id="rId9"/>
-    <sheet name="Sheet1" sheetId="9" r:id="rId10"/>
+    <sheet name="cross_over" sheetId="9" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="120">
   <si>
     <t>Seed</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1836,22 +1836,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>L=30000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>P=20</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MEAN TIME</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>run time</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>动态=40000</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1870,6 +1854,94 @@
   <si>
     <t>Time (tt*0.6)</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">population: 0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Solution: 0 3 1 0 2 1 2 0 2 1 2 0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Partition index: 0 0 0 1 0 1 1 2 2 2 3 3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">partition: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 3 7 11 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 5 9 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 6 8 10 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">color nums: 4 3 4 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">population: 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Solution: 3 0 2 0 1 2 2 0 3 3 1 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Partition index: 0 0 0 1 0 1 2 2 1 2 1 2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 3 7 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 10 11 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 5 6 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 8 9 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">color nums: 3 3 3 3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Solution: 0 3 1 0 2 1 1 0 2 1 2 0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Partition index: 0 0 0 1 0 1 2 2 1 3 2 3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 5 6 9 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 8 10 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">color nums: 4 4 3 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">c1 structure: </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">c2 structure: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Solution: 3 0 2 0 1 2 1 0 1 0 1 3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Partition index: 0 0 0 1 0 1 1 2 2 3 3 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 3 7 9 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 5 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 11 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">color nums: 4 4 2 2 </t>
   </si>
 </sst>
 </file>
@@ -2251,7 +2323,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J98"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
@@ -2283,7 +2355,7 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -3186,7 +3258,7 @@
         <v>55</v>
       </c>
       <c r="H74" s="2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="I74" t="s">
         <v>82</v>
@@ -3590,200 +3662,175 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ED288E8-003C-4A82-BC01-BAAF7FCF3F70}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="9" style="9" customWidth="1"/>
+    <col min="1" max="1" width="33.88671875" customWidth="1"/>
+    <col min="2" max="2" width="33.33203125" style="9" customWidth="1"/>
     <col min="3" max="3" width="4" customWidth="1"/>
     <col min="4" max="4" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1">
-        <v>500.1</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="D1">
-        <v>500.5</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>89</v>
-      </c>
+      <c r="A1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E1" s="9"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="D2" t="s">
-        <v>87</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>86</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="B2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E2" s="9"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B3" s="9">
-        <v>23.421099999999999</v>
-      </c>
-      <c r="D3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E3" s="9">
-        <v>40.042099999999998</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="B3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E3" s="9"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B4" s="9">
-        <v>29.711300000000001</v>
-      </c>
-      <c r="D4" t="s">
-        <v>53</v>
-      </c>
-      <c r="E4" s="9">
-        <v>15.4536</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="B4" t="s">
+        <v>94</v>
+      </c>
+      <c r="E4" s="9"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B5" s="9">
-        <v>38.357199999999999</v>
-      </c>
-      <c r="D5" t="s">
-        <v>53</v>
-      </c>
-      <c r="E5" s="9">
-        <v>25.2683</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="B5" t="s">
+        <v>102</v>
+      </c>
+      <c r="E5" s="9"/>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>53</v>
-      </c>
-      <c r="B6" s="9">
-        <v>53.893599999999999</v>
-      </c>
-      <c r="D6" t="s">
-        <v>53</v>
-      </c>
-      <c r="E6" s="9">
-        <v>34.0242</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="B6" t="s">
+        <v>103</v>
+      </c>
+      <c r="E6" s="9"/>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>53</v>
-      </c>
-      <c r="B7" s="9">
-        <v>23.152799999999999</v>
-      </c>
-      <c r="D7" t="s">
-        <v>53</v>
-      </c>
-      <c r="E7" s="9">
-        <v>16.625399999999999</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="B7" t="s">
+        <v>104</v>
+      </c>
+      <c r="E7" s="9"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" t="s">
-        <v>53</v>
-      </c>
-      <c r="B8" s="9">
-        <v>30.468499999999999</v>
-      </c>
-      <c r="D8" t="s">
-        <v>53</v>
-      </c>
-      <c r="E8" s="9">
-        <v>39.71</v>
-      </c>
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>105</v>
+      </c>
+      <c r="E8" s="9"/>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>53</v>
-      </c>
-      <c r="B9" s="9">
-        <v>56.275700000000001</v>
-      </c>
-      <c r="D9" t="s">
-        <v>53</v>
-      </c>
-      <c r="E9" s="9">
-        <v>33.592799999999997</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="B9" t="s">
+        <v>106</v>
+      </c>
+      <c r="E9" s="9"/>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>53</v>
-      </c>
-      <c r="B10" s="9">
-        <v>10.775</v>
-      </c>
-      <c r="D10" t="s">
-        <v>53</v>
-      </c>
-      <c r="E10" s="9">
-        <v>36.534100000000002</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="E10" s="9"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>53</v>
-      </c>
-      <c r="B11" s="9">
-        <v>50.822000000000003</v>
-      </c>
-      <c r="D11" t="s">
-        <v>53</v>
-      </c>
-      <c r="E11" s="9">
-        <v>26.8337</v>
-      </c>
+        <v>107</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="E11" s="9"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>53</v>
-      </c>
-      <c r="B12" s="9">
-        <v>14.825100000000001</v>
-      </c>
-      <c r="D12" t="s">
-        <v>53</v>
-      </c>
-      <c r="E12" s="9">
-        <v>44.168500000000002</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="E12" s="9"/>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>88</v>
-      </c>
-      <c r="B13" s="9">
-        <v>35.208577777777776</v>
-      </c>
-      <c r="D13" t="s">
-        <v>88</v>
-      </c>
-      <c r="E13" s="9">
-        <v>31.225269999999995</v>
+        <v>94</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="E13" s="9"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>95</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>109</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>110</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>111</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -4763,10 +4810,10 @@
         <v>84</v>
       </c>
       <c r="F14" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="G14" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -4930,10 +4977,10 @@
         <v>84</v>
       </c>
       <c r="F27" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="G27" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -5493,7 +5540,7 @@
         <v>79</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="I40" s="2" t="s">
         <v>85</v>
@@ -5635,7 +5682,7 @@
         <v>79</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="I53" s="2" t="s">
         <v>85</v>

</xml_diff>

<commit_message>
add 500.1 and 500.9
</commit_message>
<xml_diff>
--- a/npbenchmark-main/tabucol_vector/tabu_result.xlsx
+++ b/npbenchmark-main/tabucol_vector/tabu_result.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\npbenchmark\npbenchmark-main\tabucol_vector\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F97F914-0C25-4662-AF87-0F9F18A4EBD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9774F689-CC33-4995-9CEC-4EA2885F537D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="500.1" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="127">
   <si>
     <t>Seed</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1963,6 +1963,10 @@
   </si>
   <si>
     <t>max_iter=4000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>max_iter=8000</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2345,7 +2349,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A103" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="E115" sqref="E115"/>
     </sheetView>
   </sheetViews>
@@ -4155,10 +4159,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECD6EFFC-BA4E-4954-8C8C-5C7E8E2EF2DD}">
-  <dimension ref="A1:E75"/>
+  <dimension ref="A1:E89"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A75" sqref="A75"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C89" sqref="C89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -5044,6 +5048,133 @@
         <v>5.5214900000000009</v>
       </c>
     </row>
+    <row r="78" spans="1:3">
+      <c r="A78" t="s">
+        <v>120</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" t="s">
+        <v>124</v>
+      </c>
+      <c r="B79">
+        <v>1</v>
+      </c>
+      <c r="C79" s="2">
+        <v>21.550599999999999</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" t="s">
+        <v>124</v>
+      </c>
+      <c r="B80">
+        <v>2</v>
+      </c>
+      <c r="C80" s="2">
+        <v>5.8128500000000001</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" t="s">
+        <v>123</v>
+      </c>
+      <c r="B81">
+        <v>3</v>
+      </c>
+      <c r="C81" s="2">
+        <v>4.0119899999999999</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" t="s">
+        <v>123</v>
+      </c>
+      <c r="B82">
+        <v>4</v>
+      </c>
+      <c r="C82" s="1">
+        <v>10.306900000000001</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83" t="s">
+        <v>123</v>
+      </c>
+      <c r="B83">
+        <v>5</v>
+      </c>
+      <c r="C83" s="1">
+        <v>2.9172199999999999</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84" t="s">
+        <v>123</v>
+      </c>
+      <c r="B84">
+        <v>6</v>
+      </c>
+      <c r="C84" s="1">
+        <v>2.9496799999999999</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85" t="s">
+        <v>123</v>
+      </c>
+      <c r="B85">
+        <v>7</v>
+      </c>
+      <c r="C85" s="1">
+        <v>7.01403</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86" t="s">
+        <v>123</v>
+      </c>
+      <c r="B86">
+        <v>8</v>
+      </c>
+      <c r="C86" s="1">
+        <v>7.3122400000000001</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87" t="s">
+        <v>123</v>
+      </c>
+      <c r="B87">
+        <v>9</v>
+      </c>
+      <c r="C87" s="1">
+        <v>2.8584499999999999</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88" t="s">
+        <v>123</v>
+      </c>
+      <c r="B88">
+        <v>10</v>
+      </c>
+      <c r="C88" s="1">
+        <v>4.9146700000000001</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="A89" t="s">
+        <v>61</v>
+      </c>
+      <c r="C89" s="1">
+        <f>AVERAGE(C79:C88)</f>
+        <v>6.9648630000000011</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5055,7 +5186,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4A64073-A659-4E0B-A57C-5317A7C4EDA7}">
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
@@ -8483,7 +8614,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>

</xml_diff>